<commit_message>
upload pic and dte pending
</commit_message>
<xml_diff>
--- a/testdata/Tutor addevent.xlsx
+++ b/testdata/Tutor addevent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoges\PycharmProjects\ilrnu\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A32C74-85A4-4618-8CB1-5D0602F73BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E65FD0-F473-4E96-B831-38A84B332AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Online</t>
   </si>
@@ -29,12 +29,6 @@
     <t>Offline</t>
   </si>
   <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>Dance</t>
-  </si>
-  <si>
     <t>Music classes</t>
   </si>
   <si>
@@ -141,13 +135,22 @@
   </si>
   <si>
     <t>Actualresult</t>
+  </si>
+  <si>
+    <t>sports</t>
+  </si>
+  <si>
+    <t>dance</t>
+  </si>
+  <si>
+    <t>./testdata/Maths.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +181,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -282,6 +291,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,7 +639,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" style="7" bestFit="1" customWidth="1"/>
@@ -645,65 +657,65 @@
     <col min="15" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" s="10" customFormat="1" ht="72">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
       </c>
       <c r="F2" s="12">
         <v>44218</v>
@@ -721,31 +733,31 @@
         <v>15</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="10" customFormat="1" ht="43.2">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" s="12">
         <v>44219</v>
@@ -763,13 +775,13 @@
         <v>30</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N3" s="9"/>
     </row>
@@ -787,14 +799,14 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:17">
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -807,7 +819,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:17">
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -815,15 +827,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:17">
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -837,15 +849,15 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:17">
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -859,15 +871,15 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:17">
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" s="4">
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -881,15 +893,15 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:17">
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" s="4">
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -903,15 +915,15 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:17">
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2">
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -925,15 +937,15 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:17">
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="4">
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -947,15 +959,15 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:17">
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="4">
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -969,15 +981,15 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:17">
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E13" s="4">
         <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -991,15 +1003,15 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:17">
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" s="4">
         <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1013,15 +1025,15 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:17">
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="4">
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1035,15 +1047,15 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:17">
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="4">
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1057,15 +1069,15 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:17">
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1">
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1079,12 +1091,12 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:17">
       <c r="D18" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload pic complete and dte pending
</commit_message>
<xml_diff>
--- a/testdata/Tutor addevent.xlsx
+++ b/testdata/Tutor addevent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoges\PycharmProjects\ilrnu\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E65FD0-F473-4E96-B831-38A84B332AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EE3B6B-8650-49B7-9F36-ADE1B53442B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Online</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Picture</t>
   </si>
   <si>
-    <t>"P:\iLRNU application\Testdata\Maths.jpg"</t>
-  </si>
-  <si>
     <t>Expected</t>
   </si>
   <si>
@@ -143,14 +140,14 @@
     <t>dance</t>
   </si>
   <si>
-    <t>./testdata/Maths.jpg</t>
+    <t>"P://iLRNU application//Testdata//Maths.jpg"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,12 +178,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -254,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -291,9 +282,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,10 +624,10 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" style="7" bestFit="1" customWidth="1"/>
@@ -657,56 +645,56 @@
     <col min="15" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>23</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="72">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="10" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>2</v>
@@ -735,20 +723,20 @@
       <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>40</v>
+      <c r="L2" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" ht="43.2">
+    <row r="3" spans="1:14" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>3</v>
@@ -778,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>8</v>
@@ -799,14 +787,14 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:17">
+    <row r="4" spans="4:17" x14ac:dyDescent="0.3">
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -819,7 +807,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="4:17">
+    <row r="5" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -827,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:17">
+    <row r="6" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -849,7 +837,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="4:17">
+    <row r="7" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
@@ -871,7 +859,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="4:17">
+    <row r="8" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
@@ -893,7 +881,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="4:17">
+    <row r="9" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
@@ -915,7 +903,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="4:17">
+    <row r="10" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
@@ -937,7 +925,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="4:17">
+    <row r="11" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
@@ -959,7 +947,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="4:17">
+    <row r="12" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
@@ -981,7 +969,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="4:17">
+    <row r="13" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1003,7 +991,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="4:17">
+    <row r="14" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1025,7 +1013,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="4:17">
+    <row r="15" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1047,7 +1035,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="4:17">
+    <row r="16" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1069,7 +1057,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="4:17">
+    <row r="17" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +1079,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="4:17">
+    <row r="18" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D18" s="5" t="s">
         <v>22</v>
       </c>

</xml_diff>